<commit_message>
added test data for import, updated import functions to fix errors, and updated function examples
</commit_message>
<xml_diff>
--- a/inst/extdata/sample_rb.xlsx
+++ b/inst/extdata/sample_rb.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shmer\Dropbox\My Documents\writeAlizer\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{276A3F3B-9E8C-452A-9A58-8A09A0BA33B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F72D4FA-5504-4B4E-988C-9733ECD3DF49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1590" yWindow="345" windowWidth="11700" windowHeight="11385"/>
+    <workbookView xWindow="11460" yWindow="1725" windowWidth="11700" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="sample_rb" sheetId="1" r:id="rId1"/>
+    <sheet name="oz_rb" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="1319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="1316">
   <si>
     <t>File name</t>
   </si>
@@ -3968,21 +3968,12 @@
   </si>
   <si>
     <t>RB.AvgWordsListSen_They_LIWC</t>
-  </si>
-  <si>
-    <t>page7</t>
-  </si>
-  <si>
-    <t>page8</t>
-  </si>
-  <si>
-    <t>page9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4816,10 +4807,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AXP4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -8774,8 +8767,8 @@
       </c>
     </row>
     <row r="2" spans="1:1316" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1316</v>
+      <c r="A2">
+        <v>7</v>
       </c>
       <c r="B2">
         <v>11</v>
@@ -12724,8 +12717,8 @@
       </c>
     </row>
     <row r="3" spans="1:1316" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1317</v>
+      <c r="A3">
+        <v>8</v>
       </c>
       <c r="B3">
         <v>13</v>
@@ -16674,8 +16667,8 @@
       </c>
     </row>
     <row r="4" spans="1:1316" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1318</v>
+      <c r="A4">
+        <v>9</v>
       </c>
       <c r="B4">
         <v>17</v>

</xml_diff>